<commit_message>
My EDA2 now gives me the template
</commit_message>
<xml_diff>
--- a/CH-085 Custome Ranking.xlsx
+++ b/CH-085 Custome Ranking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C314460D-DF8A-4B62-B9CB-A02465C8F9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398D35BE-211F-4D1D-9B16-D078CCDEB3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{F722F3FF-1085-48CD-AB15-9E26505C6112}"/>
   </bookViews>
@@ -963,16 +963,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>18</xdr:col>
-          <xdr:colOff>1270</xdr:colOff>
-          <xdr:row>26</xdr:row>
-          <xdr:rowOff>2540</xdr:rowOff>
+          <xdr:col>20</xdr:col>
+          <xdr:colOff>248920</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>85090</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>21</xdr:col>
-          <xdr:colOff>529590</xdr:colOff>
-          <xdr:row>46</xdr:row>
-          <xdr:rowOff>184150</xdr:rowOff>
+          <xdr:col>24</xdr:col>
+          <xdr:colOff>62230</xdr:colOff>
+          <xdr:row>45</xdr:row>
+          <xdr:rowOff>67310</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -987,7 +987,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$E$3:$F$23" spid="_x0000_s6148"/>
+                  <a14:cameraTool cellRange="$E$3:$F$23" spid="_x0000_s6149"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1001,8 +1001,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="16200120" y="5285740"/>
-              <a:ext cx="2677160" cy="4241800"/>
+              <a:off x="17882870" y="4961890"/>
+              <a:ext cx="2680970" cy="4248150"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -22185,8 +22185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164D1AE9-9669-449D-9482-07FFFB82CC8C}">
   <dimension ref="A1:Y988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J35" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -22437,7 +22437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="43">
         <v>60</v>
       </c>
@@ -22449,7 +22449,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="42">
         <v>63</v>
       </c>
@@ -22461,7 +22461,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="41">
         <v>64</v>
       </c>
@@ -22473,7 +22473,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="40">
         <v>67</v>
       </c>
@@ -22485,7 +22485,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="39">
         <v>68</v>
       </c>
@@ -22497,7 +22497,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="38">
         <v>69</v>
       </c>
@@ -22509,7 +22509,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="37">
         <v>74</v>
       </c>
@@ -22521,19 +22521,19 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="32"/>
       <c r="E24" s="46"/>
     </row>
-    <row r="25" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="32"/>
       <c r="E25" s="46"/>
     </row>
-    <row r="26" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="47"/>
       <c r="E26" s="46"/>
     </row>
-    <row r="27" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="47"/>
       <c r="C27" s="53" cm="1">
         <f t="array" ref="C27:D38">_xlfn.LET(
@@ -22555,11 +22555,11 @@
         <v>1</v>
       </c>
       <c r="I27" s="27">
-        <f>IF(F27&lt;G27,C27,D27)</f>
+        <f>IF(F27&lt;IFERROR(G27,100),C27,D27)</f>
         <v>51</v>
       </c>
       <c r="J27" s="27">
-        <f>IF(F27&lt;G27,D27,C27)</f>
+        <f>IF(F27&lt;IFERROR(G27,100),D27,C27)</f>
         <v>47</v>
       </c>
       <c r="L27" s="27" cm="1">
@@ -22576,8 +22576,15 @@
       <c r="P27" s="27">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R27" s="27" t="b" cm="1">
+        <f t="array" ref="R27:S47">_xlfn.ANCHORARRAY(O27)=E3:F23</f>
+        <v>1</v>
+      </c>
+      <c r="S27" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="47"/>
       <c r="C28" s="53">
         <v>45</v>
@@ -22593,11 +22600,11 @@
         <v>2</v>
       </c>
       <c r="I28" s="27">
-        <f t="shared" ref="I28:I35" si="0">IF(F28&lt;G28,C28,D28)</f>
+        <f t="shared" ref="I28:I38" si="0">IF(F28&lt;IFERROR(G28,100),C28,D28)</f>
         <v>52</v>
       </c>
       <c r="J28" s="27">
-        <f t="shared" ref="J28:J35" si="1">IF(F28&lt;G28,D28,C28)</f>
+        <f t="shared" ref="J28:J38" si="1">IF(F28&lt;IFERROR(G28,100),D28,C28)</f>
         <v>45</v>
       </c>
       <c r="L28" s="27">
@@ -22612,8 +22619,14 @@
       <c r="P28" s="27">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R28" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S28" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="47"/>
       <c r="C29" s="53">
         <v>44</v>
@@ -22648,8 +22661,14 @@
       <c r="P29" s="27">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R29" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S29" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="47"/>
       <c r="C30" s="53">
         <v>43</v>
@@ -22684,8 +22703,14 @@
       <c r="P30" s="27">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R30" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S30" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="47"/>
       <c r="C31" s="53">
         <v>42</v>
@@ -22720,8 +22745,14 @@
       <c r="P31" s="27">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R31" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S31" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="47"/>
       <c r="C32" s="53">
         <v>40</v>
@@ -22756,8 +22787,14 @@
       <c r="P32" s="27">
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R32" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S32" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="47"/>
       <c r="C33" s="53">
         <v>34</v>
@@ -22792,8 +22829,14 @@
       <c r="P33" s="27">
         <v>11</v>
       </c>
-    </row>
-    <row r="34" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R33" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S33" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="47"/>
       <c r="C34" s="53">
         <v>30</v>
@@ -22828,8 +22871,14 @@
       <c r="P34" s="27">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R34" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S34" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="47"/>
       <c r="C35" s="53">
         <v>28</v>
@@ -22864,8 +22913,14 @@
       <c r="P35" s="27">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R35" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S35" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="47"/>
       <c r="C36" s="53">
         <v>27</v>
@@ -22880,11 +22935,12 @@
       <c r="G36" s="27" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I36" s="53">
+      <c r="I36" s="27">
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="J36" s="27" t="e">
-        <f t="shared" ref="J28:J38" si="2">IF(F36&lt;G36,D36,C36)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="L36" s="27">
@@ -22899,8 +22955,14 @@
       <c r="P36" s="27">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R36" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S36" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="47"/>
       <c r="C37" s="53">
         <v>25</v>
@@ -22915,11 +22977,12 @@
       <c r="G37" s="27" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I37" s="53">
+      <c r="I37" s="27">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="J37" s="27" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="L37" s="27">
@@ -22934,8 +22997,14 @@
       <c r="P37" s="27">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R37" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S37" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="47"/>
       <c r="C38" s="53">
         <v>22</v>
@@ -22950,11 +23019,12 @@
       <c r="G38" s="27" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I38" s="53">
+      <c r="I38" s="27">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="J38" s="27" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="L38" s="27">
@@ -22969,8 +23039,14 @@
       <c r="P38" s="27">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R38" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S38" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="47"/>
       <c r="E39" s="46"/>
       <c r="L39" s="27">
@@ -22985,8 +23061,14 @@
       <c r="P39" s="27">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R39" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S39" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="47"/>
       <c r="C40" s="27" cm="1">
         <f t="array" ref="C40:C60">_xlfn.LET(
@@ -23016,8 +23098,14 @@
       <c r="P40" s="27">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R40" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S40" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="47"/>
       <c r="C41" s="27">
         <v>51</v>
@@ -23038,8 +23126,14 @@
       <c r="P41" s="27">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R41" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S41" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="47"/>
       <c r="C42" s="27">
         <v>45</v>
@@ -23060,8 +23154,14 @@
       <c r="P42" s="27">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R42" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S42" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="47"/>
       <c r="C43" s="27">
         <v>52</v>
@@ -23082,8 +23182,14 @@
       <c r="P43" s="27">
         <v>10</v>
       </c>
-    </row>
-    <row r="44" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R43" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S43" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="47"/>
       <c r="C44" s="27">
         <v>44</v>
@@ -23104,8 +23210,14 @@
       <c r="P44" s="27">
         <v>12</v>
       </c>
-    </row>
-    <row r="45" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R44" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S44" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="47"/>
       <c r="C45" s="27">
         <v>60</v>
@@ -23126,8 +23238,14 @@
       <c r="P45" s="27">
         <v>14</v>
       </c>
-    </row>
-    <row r="46" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R45" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S45" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="47"/>
       <c r="C46" s="27">
         <v>43</v>
@@ -23148,8 +23266,14 @@
       <c r="P46" s="27">
         <v>15</v>
       </c>
-    </row>
-    <row r="47" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R46" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S46" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="47"/>
       <c r="C47" s="27">
         <v>63</v>
@@ -23170,8 +23294,14 @@
       <c r="P47" s="27">
         <v>18</v>
       </c>
-    </row>
-    <row r="48" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R47" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="S47" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="47"/>
       <c r="C48" s="27">
         <v>42</v>

</xml_diff>

<commit_message>
Finally, I got my single function working
</commit_message>
<xml_diff>
--- a/CH-085 Custome Ranking.xlsx
+++ b/CH-085 Custome Ranking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF764B3B-CD9E-462E-BDAB-B0434301359F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B207AB-45A4-47B2-8686-E1591F75F5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{F722F3FF-1085-48CD-AB15-9E26505C6112}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="9">
   <si>
     <t>Question</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>disb</t>
+  </si>
+  <si>
+    <t>Single Function</t>
   </si>
 </sst>
 </file>
@@ -988,7 +991,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$E$3:$F$23" spid="_x0000_s6150"/>
+                  <a14:cameraTool cellRange="$E$3:$F$23" spid="_x0000_s6151"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1059,7 +1062,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$E$3:$F$23" spid="_x0000_s7169"/>
+                  <a14:cameraTool cellRange="$E$3:$F$23" spid="_x0000_s7170"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -27360,8 +27363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CFB637-46D5-4A2C-9F34-88617D1E5A47}">
   <dimension ref="A1:Y988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F22" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28203,6 +28206,8 @@
     </row>
     <row r="39" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="47"/>
+      <c r="C39"/>
+      <c r="D39"/>
       <c r="E39" s="46"/>
       <c r="L39" s="27">
         <v>34</v>
@@ -28225,21 +28230,8 @@
     </row>
     <row r="40" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="47"/>
-      <c r="C40" s="27" cm="1">
-        <f t="array" ref="C40:C60">_xlfn.LET(
-_xlpm.z,_xlfn.TOCOL(_xlfn.ANCHORARRAY(C27),3),
-_xlpm.zz,_xlfn.HSTACK(_xlpm.z,
-          _xlfn.SORTBY(_xlfn.SEQUENCE(ROWS(_xlpm.z)),
-                 _xlfn.XMATCH(_xlpm.z,B3:B23)
-          )),
-_xlpm.z
-)</f>
-        <v>47</v>
-      </c>
-      <c r="D40" s="27" cm="1">
-        <f t="array" ref="D40:D60">_xlfn.SEQUENCE(21)</f>
-        <v>1</v>
-      </c>
+      <c r="C40"/>
+      <c r="D40"/>
       <c r="E40" s="46"/>
       <c r="L40" s="27">
         <v>68</v>
@@ -28262,12 +28254,8 @@
     </row>
     <row r="41" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="47"/>
-      <c r="C41" s="27">
-        <v>51</v>
-      </c>
-      <c r="D41" s="27">
-        <v>2</v>
-      </c>
+      <c r="C41"/>
+      <c r="D41"/>
       <c r="E41" s="46"/>
       <c r="L41" s="27">
         <v>69</v>
@@ -28290,12 +28278,8 @@
     </row>
     <row r="42" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="47"/>
-      <c r="C42" s="27">
-        <v>45</v>
-      </c>
-      <c r="D42" s="27">
-        <v>3</v>
-      </c>
+      <c r="C42"/>
+      <c r="D42"/>
       <c r="E42" s="46"/>
       <c r="L42" s="27">
         <v>30</v>
@@ -28318,11 +28302,8 @@
     </row>
     <row r="43" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="47"/>
-      <c r="C43" s="27">
-        <v>52</v>
-      </c>
-      <c r="D43" s="27">
-        <v>4</v>
+      <c r="C43" s="27" t="s">
+        <v>8</v>
       </c>
       <c r="E43" s="46"/>
       <c r="L43" s="27">
@@ -28346,11 +28327,23 @@
     </row>
     <row r="44" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="47"/>
-      <c r="C44" s="27">
-        <v>44</v>
+      <c r="C44" s="27" cm="1">
+        <f t="array" ref="C44:D64">_xlfn.LET(
+_xlpm.a, B3:B23,
+_xlpm.fl, _xlfn.LAMBDA(_xlpm.x, _xlfn._xlws.SORT(_xlfn._xlws.FILTER(_xlpm.a, IF(_xlpm.x = -1, _xlpm.a &lt; 50, IF(_xlpm.x = 1, _xlpm.a &gt; 50))), 1, _xlpm.x)),
+_xlpm.z, _xlfn.HSTACK(_xlpm.fl(-1),_xlpm.fl(1)),
+_xlpm.zz, ABS(_xlpm.z-50),
+_xlpm.zzz1, IF(_xlfn.CHOOSECOLS(_xlpm.zz,1)&lt;IFERROR(_xlfn.CHOOSECOLS(_xlpm.zz,2),100),_xlfn.CHOOSECOLS(_xlpm.z,1),_xlfn.CHOOSECOLS(_xlpm.z,2)),
+_xlpm.zzz2, IF(_xlfn.CHOOSECOLS(_xlpm.zz,1)&lt;IFERROR(_xlfn.CHOOSECOLS(_xlpm.zz,2),100),_xlfn.CHOOSECOLS(_xlpm.z,2),_xlfn.CHOOSECOLS(_xlpm.z,1)),
+_xlpm.zzz, _xlfn.HSTACK(_xlpm.zzz1,_xlpm.zzz2),
+_xlpm.zzzz1, _xlfn.TOCOL(_xlpm.zzz,3),
+_xlpm.zzzz, _xlfn.HSTACK(_xlpm.zzzz1,_xlfn.SEQUENCE(ROWS(_xlpm.zzzz1))),
+_xlfn.SORTBY(_xlpm.zzzz,_xlfn.XMATCH(_xlfn.CHOOSECOLS(_xlpm.zzzz,1),B3:B23))
+)</f>
+        <v>22</v>
       </c>
       <c r="D44" s="27">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E44" s="46"/>
       <c r="L44" s="27">
@@ -28375,10 +28368,10 @@
     <row r="45" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="47"/>
       <c r="C45" s="27">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="D45" s="27">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E45" s="46"/>
       <c r="L45" s="27">
@@ -28403,10 +28396,10 @@
     <row r="46" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="47"/>
       <c r="C46" s="27">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="D46" s="27">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E46" s="46"/>
       <c r="L46" s="27">
@@ -28431,10 +28424,10 @@
     <row r="47" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="47"/>
       <c r="C47" s="27">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="D47" s="27">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E47" s="46"/>
       <c r="L47" s="27">
@@ -28459,20 +28452,20 @@
     <row r="48" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="47"/>
       <c r="C48" s="27">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D48" s="27">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E48" s="46"/>
     </row>
     <row r="49" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="47"/>
       <c r="C49" s="27">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="D49" s="27">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E49" s="46"/>
     </row>
@@ -28489,320 +28482,217 @@
     <row r="51" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="47"/>
       <c r="C51" s="27">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D51" s="27">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E51" s="46"/>
     </row>
     <row r="52" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="47"/>
       <c r="C52" s="27">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D52" s="27">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E52" s="46"/>
     </row>
     <row r="53" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="47"/>
       <c r="C53" s="27">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D53" s="27">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E53" s="46"/>
     </row>
     <row r="54" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="47"/>
       <c r="C54" s="27">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D54" s="27">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E54" s="46"/>
     </row>
     <row r="55" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="47"/>
       <c r="C55" s="27">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="D55" s="27">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E55" s="46"/>
     </row>
     <row r="56" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="47"/>
       <c r="C56" s="27">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="D56" s="27">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E56" s="46"/>
     </row>
     <row r="57" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="47"/>
       <c r="C57" s="27">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="D57" s="27">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E57" s="46"/>
     </row>
     <row r="58" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="47"/>
       <c r="C58" s="27">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="D58" s="27">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E58" s="46"/>
     </row>
     <row r="59" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="47"/>
       <c r="C59" s="27">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="D59" s="27">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E59" s="46"/>
     </row>
     <row r="60" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="47"/>
       <c r="C60" s="27">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="D60" s="27">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E60" s="46"/>
     </row>
     <row r="61" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="47"/>
+      <c r="C61" s="27">
+        <v>67</v>
+      </c>
+      <c r="D61" s="27">
+        <v>12</v>
+      </c>
       <c r="E61" s="46"/>
     </row>
     <row r="62" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="47"/>
+      <c r="C62" s="27">
+        <v>68</v>
+      </c>
+      <c r="D62" s="27">
+        <v>14</v>
+      </c>
       <c r="E62" s="46"/>
     </row>
     <row r="63" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="47"/>
-      <c r="C63" s="27" cm="1">
-        <f t="array" ref="C63:D83">_xlfn.LET(_xlpm.z,C40:D60,_xlfn.SORTBY(_xlpm.z,_xlfn.XMATCH(_xlfn.CHOOSECOLS(_xlpm.z,1),B3:B23)))</f>
-        <v>22</v>
+      <c r="C63" s="27">
+        <v>69</v>
       </c>
       <c r="D63" s="27">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E63" s="46"/>
     </row>
     <row r="64" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="47"/>
       <c r="C64" s="27">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="D64" s="27">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E64" s="46"/>
     </row>
     <row r="65" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="47"/>
-      <c r="C65" s="27">
-        <v>27</v>
-      </c>
-      <c r="D65" s="27">
-        <v>19</v>
-      </c>
       <c r="E65" s="46"/>
     </row>
     <row r="66" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="47"/>
-      <c r="C66" s="27">
-        <v>28</v>
-      </c>
-      <c r="D66" s="27">
-        <v>17</v>
-      </c>
       <c r="E66" s="46"/>
     </row>
     <row r="67" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="47"/>
-      <c r="C67" s="27">
-        <v>30</v>
-      </c>
-      <c r="D67" s="27">
-        <v>15</v>
-      </c>
       <c r="E67" s="46"/>
     </row>
     <row r="68" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="47"/>
-      <c r="C68" s="27">
-        <v>34</v>
-      </c>
-      <c r="D68" s="27">
-        <v>13</v>
-      </c>
       <c r="E68" s="46"/>
     </row>
     <row r="69" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="47"/>
-      <c r="C69" s="27">
-        <v>40</v>
-      </c>
-      <c r="D69" s="27">
-        <v>11</v>
-      </c>
       <c r="E69" s="46"/>
     </row>
     <row r="70" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="47"/>
-      <c r="C70" s="27">
-        <v>42</v>
-      </c>
-      <c r="D70" s="27">
-        <v>9</v>
-      </c>
       <c r="E70" s="46"/>
     </row>
     <row r="71" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="47"/>
-      <c r="C71" s="27">
-        <v>43</v>
-      </c>
-      <c r="D71" s="27">
-        <v>7</v>
-      </c>
       <c r="E71" s="46"/>
     </row>
     <row r="72" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="47"/>
-      <c r="C72" s="27">
-        <v>44</v>
-      </c>
-      <c r="D72" s="27">
-        <v>5</v>
-      </c>
       <c r="E72" s="46"/>
     </row>
     <row r="73" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="47"/>
-      <c r="C73" s="27">
-        <v>45</v>
-      </c>
-      <c r="D73" s="27">
-        <v>3</v>
-      </c>
       <c r="E73" s="46"/>
     </row>
     <row r="74" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="47"/>
-      <c r="C74" s="27">
-        <v>47</v>
-      </c>
-      <c r="D74" s="27">
-        <v>1</v>
-      </c>
       <c r="E74" s="46"/>
     </row>
     <row r="75" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="47"/>
-      <c r="C75" s="27">
-        <v>51</v>
-      </c>
-      <c r="D75" s="27">
-        <v>2</v>
-      </c>
       <c r="E75" s="46"/>
     </row>
     <row r="76" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="47"/>
-      <c r="C76" s="27">
-        <v>52</v>
-      </c>
-      <c r="D76" s="27">
-        <v>4</v>
-      </c>
       <c r="E76" s="46"/>
     </row>
     <row r="77" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="47"/>
-      <c r="C77" s="27">
-        <v>60</v>
-      </c>
-      <c r="D77" s="27">
-        <v>6</v>
-      </c>
       <c r="E77" s="46"/>
     </row>
     <row r="78" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" s="47"/>
-      <c r="C78" s="27">
-        <v>63</v>
-      </c>
-      <c r="D78" s="27">
-        <v>8</v>
-      </c>
       <c r="E78" s="46"/>
     </row>
     <row r="79" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="47"/>
-      <c r="C79" s="27">
-        <v>64</v>
-      </c>
-      <c r="D79" s="27">
-        <v>10</v>
-      </c>
       <c r="E79" s="46"/>
     </row>
     <row r="80" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="47"/>
-      <c r="C80" s="27">
-        <v>67</v>
-      </c>
-      <c r="D80" s="27">
-        <v>12</v>
-      </c>
       <c r="E80" s="46"/>
     </row>
     <row r="81" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" s="47"/>
-      <c r="C81" s="27">
-        <v>68</v>
-      </c>
-      <c r="D81" s="27">
-        <v>14</v>
-      </c>
       <c r="E81" s="46"/>
     </row>
     <row r="82" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="47"/>
-      <c r="C82" s="27">
-        <v>69</v>
-      </c>
-      <c r="D82" s="27">
-        <v>16</v>
-      </c>
       <c r="E82" s="46"/>
     </row>
     <row r="83" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="47"/>
-      <c r="C83" s="27">
-        <v>74</v>
-      </c>
-      <c r="D83" s="27">
-        <v>18</v>
-      </c>
       <c r="E83" s="46"/>
     </row>
     <row r="84" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>